<commit_message>
Additional Test added with custom extent report
</commit_message>
<xml_diff>
--- a/DemoWiniumProj/src/main/java/com/qa/report/SceintificCal_testdata.xlsx
+++ b/DemoWiniumProj/src/main/java/com/qa/report/SceintificCal_testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\MyCode\Winium\DemoWiniumProj\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CE4AB2B7-87BF-4929-95E2-8586483C5391}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C41B4C3C-AF0E-48BF-AB0D-32C85C36C59D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="10890" windowWidth="20460" xWindow="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="30"/>
+    <workbookView activeTab="1" windowHeight="10890" windowWidth="20460" xWindow="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="testdata" r:id="rId1" sheetId="1"/>
+    <sheet name="execution" r:id="rId1" sheetId="2"/>
+    <sheet name="testdata" r:id="rId2" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>FirstNumber</t>
   </si>
@@ -77,73 +78,91 @@
     <t>4</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:40:57</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:04</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:12</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:19</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:27</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:35</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:42</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:50</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:41:58</t>
-  </si>
-  <si>
     <t>ExpectedResult</t>
   </si>
   <si>
-    <t>2019/11/10 19:45:38</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:45:46</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:45:53</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:01</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:09</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:16</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:24</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:31</t>
-  </si>
-  <si>
-    <t>2019/11/10 19:46:39</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>2019/11/15 10:21:35</t>
+  </si>
+  <si>
+    <t>2019/11/15 10:21:43</t>
+  </si>
+  <si>
+    <t>2019/11/15 10:21:52</t>
+  </si>
+  <si>
+    <t>2019/11/15 10:22:00</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Add 2 Numbers</t>
+  </si>
+  <si>
+    <t>Multiply 2 Numbers</t>
+  </si>
+  <si>
+    <t>Division 2 Numbers</t>
+  </si>
+  <si>
+    <t>Subtract 2 Numbers</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:34:03</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:34:14</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:34:24</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:34:34</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:40:23</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:40:32</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:40:41</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:40:50</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:41:14</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:41:24</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:41:33</t>
+  </si>
+  <si>
+    <t>2019/11/16 18:41:42</t>
   </si>
 </sst>
 </file>
@@ -211,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -232,6 +251,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -513,24 +538,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83F55F9-DAB2-41CA-BF56-8FEC2F3A4B88}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.76171875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.01953125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="12.5859375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="20.01953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.765625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -544,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>9</v>
@@ -552,8 +700,11 @@
       <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -574,17 +725,20 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="7">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4">
@@ -598,10 +752,13 @@
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -615,17 +772,19 @@
         <v>7</v>
       </c>
       <c r="E4" s="4">
-        <f>B4+D4</f>
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -639,134 +798,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <f>B5-D5</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4">
-        <f>B6+D6</f>
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2">
-        <f>B7*D7</f>
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4">
-        <f>B8+D8</f>
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
-        <f>B9+D9</f>
-        <v>9</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <f>B10*D10</f>
-        <v>6</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>